<commit_message>
Process completed and tested until DownloadReports.xaml in the process.xaml
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jureyes\Documents\UiPath\UiPathCertif_GenerateYearlyReport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FB0AB0-EBEE-4E9F-BAAA-8818528FEC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2D59CE-7151-49E5-B4B8-7655501808CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-9270" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -314,9 +314,6 @@
     <t>outputFolder</t>
   </si>
   <si>
-    <t>Data/Output</t>
-  </si>
-  <si>
     <t>Output folder</t>
   </si>
   <si>
@@ -345,6 +342,9 @@
   </si>
   <si>
     <t>path to upload yearly report</t>
+  </si>
+  <si>
+    <t>Data\Output</t>
   </si>
 </sst>
 </file>
@@ -401,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -411,7 +411,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -729,7 +728,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -866,13 +865,13 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -968,32 +967,32 @@
         <v>95</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>